<commit_message>
Added age to the demo
Update to data
</commit_message>
<xml_diff>
--- a/data/COPA_EHP_Demographics_Public.xlsx
+++ b/data/COPA_EHP_Demographics_Public.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -365,25 +365,30 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Group</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>PackYear</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>TimeSinceQuit</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>FEV1_FVC</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>FEV1pp</t>
         </is>
@@ -395,23 +400,26 @@
           <t>EHP01</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2">
+        <v>47</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>80</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>118</v>
       </c>
     </row>
@@ -421,23 +429,26 @@
           <t>EHP02</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3">
+        <v>51</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>77</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>106</v>
       </c>
     </row>
@@ -447,23 +458,26 @@
           <t>EHP03</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4">
+        <v>72</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0</v>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>80</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>162</v>
       </c>
     </row>
@@ -473,23 +487,26 @@
           <t>EHP04</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5">
+        <v>54</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0</v>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>79</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>120</v>
       </c>
     </row>
@@ -499,23 +516,26 @@
           <t>EHP05</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6">
+        <v>55</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0</v>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>74</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>111</v>
       </c>
     </row>
@@ -525,23 +545,26 @@
           <t>EHP06</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7">
+        <v>52</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>80</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>120</v>
       </c>
     </row>
@@ -551,23 +574,26 @@
           <t>EHP07</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8">
+        <v>63</v>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>78</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>127</v>
       </c>
     </row>
@@ -577,23 +603,26 @@
           <t>EHP08</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9">
+        <v>58</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>NS</t>
         </is>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>75</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>133</v>
       </c>
     </row>
@@ -603,23 +632,26 @@
           <t>EHP09</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10">
+        <v>56</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>ES</t>
         </is>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>50</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>8</t>
         </is>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>74</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>113</v>
       </c>
     </row>
@@ -629,23 +661,26 @@
           <t>EHP10</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11">
+        <v>50</v>
+      </c>
+      <c r="C11" t="inlineStr">
         <is>
           <t>ES</t>
         </is>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>15</v>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>79</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>106</v>
       </c>
     </row>
@@ -655,23 +690,26 @@
           <t>EHP11</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12">
+        <v>45</v>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>ES</t>
         </is>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>10.5</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>0.83</t>
         </is>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>76</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>109</v>
       </c>
     </row>
@@ -681,23 +719,26 @@
           <t>EHP12</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13">
+        <v>61</v>
+      </c>
+      <c r="C13" t="inlineStr">
         <is>
           <t>ES</t>
         </is>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>92.5</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>25</t>
         </is>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>81</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>108</v>
       </c>
     </row>
@@ -707,23 +748,26 @@
           <t>EHP13</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14">
+        <v>73</v>
+      </c>
+      <c r="C14" t="inlineStr">
         <is>
           <t>ES</t>
         </is>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>30</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>42</t>
         </is>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>86</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>120</v>
       </c>
     </row>
@@ -733,23 +777,26 @@
           <t>EHP14</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15">
+        <v>70</v>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>ES</t>
         </is>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>90</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>19</t>
         </is>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>72</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>93</v>
       </c>
     </row>
@@ -759,23 +806,26 @@
           <t>EHP15</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16">
+        <v>63</v>
+      </c>
+      <c r="C16" t="inlineStr">
         <is>
           <t>ES</t>
         </is>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>47</v>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>70</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>96.7</v>
       </c>
     </row>
@@ -785,23 +835,26 @@
           <t>EHP16</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17">
+        <v>75</v>
+      </c>
+      <c r="C17" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>7</v>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>41</t>
         </is>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>67</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>116</v>
       </c>
     </row>
@@ -811,23 +864,26 @@
           <t>EHP17</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18">
+        <v>70</v>
+      </c>
+      <c r="C18" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>19.5</v>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>64</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>88.59999999999999</v>
       </c>
     </row>
@@ -837,23 +893,26 @@
           <t>EHP18</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19">
+        <v>66</v>
+      </c>
+      <c r="C19" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>5</v>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>44</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>65.8</v>
       </c>
     </row>
@@ -863,23 +922,26 @@
           <t>EHP19</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20">
+        <v>65</v>
+      </c>
+      <c r="C20" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>3</v>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>35</t>
         </is>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>69</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>102</v>
       </c>
     </row>
@@ -889,23 +951,26 @@
           <t>EHP20</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21">
+        <v>66</v>
+      </c>
+      <c r="C21" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>67.5</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>62</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>93</v>
       </c>
     </row>
@@ -915,23 +980,26 @@
           <t>EHP21</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22">
+        <v>68</v>
+      </c>
+      <c r="C22" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>46</v>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>27</t>
         </is>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>69</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>97</v>
       </c>
     </row>
@@ -941,23 +1009,26 @@
           <t>EHP22</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B23">
+        <v>80</v>
+      </c>
+      <c r="C23" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>10</v>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>54</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>97.3</v>
       </c>
     </row>
@@ -967,23 +1038,26 @@
           <t>EHP23</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24">
+        <v>66</v>
+      </c>
+      <c r="C24" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>24</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>54</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>86</v>
       </c>
     </row>
@@ -993,23 +1067,26 @@
           <t>EHP24</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B25">
+        <v>70</v>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>12</v>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>48</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>88.3</v>
       </c>
     </row>
@@ -1019,23 +1096,26 @@
           <t>EHP25</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B26">
+        <v>67</v>
+      </c>
+      <c r="C26" t="inlineStr">
         <is>
           <t>ES-COPD</t>
         </is>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>52.5</v>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>11</t>
         </is>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>49</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>76.2</v>
       </c>
     </row>

</xml_diff>